<commit_message>
Fix Excel Data Issues, Add Error Pages, and Enhance UI
**แก้ไขข้อมูล Excel, เพิ่มหน้า Error, และปรับปรุง UI:**
- แก้ไขข้อผิดพลาดใน views.py เมื่อผู้ใช้ใส่ข้อมูล Excel ที่ไม่ใช่ประเภท string
- เพิ่มหน้า 404.html และ 500.html ใน maximo_project/templates/errors
- แก้ไขบั๊กในฟอร์มเมื่อกลับมาแล้วค่าใน dropdown ไม่แสดง
- ลบไฟล์ที่ไม่จำเป็นออก
- อัปเดท base.html
- ปรับปรุง upload_form.html ให้รองรับการแสดงผลบนหลายอุปกรณ์

**Fix Excel Data Issues, Add Error Pages, and Enhance UI:**
- Fixed error in views.py when the Excel input data is not of type string
- Added 404.html and 500.html pages in maximo_project/templates/errors
- Resolved dropdown bug in the form when returning back
- Removed unnecessary files
- Updated base.html
- Enhanced upload_form.html for responsive design
</commit_message>
<xml_diff>
--- a/static/excel/Final Schedule.xlsx
+++ b/static/excel/Final Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\narav\Downloads\maximo\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559A03C5-18AB-4888-8855-FA0644A710BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD48514-7C94-4125-BAE7-1C92F2280781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -531,7 +531,7 @@
     <author>นราวิชญ์ ชูช่วย</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{CF810A22-28C2-497C-995C-5946BDB4BD96}">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{AAE786C7-27A6-497F-B0B6-5B560C23B123}">
       <text>
         <r>
           <rPr>
@@ -596,7 +596,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{A7FE6A50-1708-4E08-8091-D755889B47F4}">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{CEEDE848-2E10-4142-BCBC-47530B9E67A9}">
       <text>
         <r>
           <rPr>
@@ -639,24 +639,40 @@
           <t xml:space="preserve">
 - ความยาวของข้อมูลห้ามเกิน 100 ตัวอักษร</t>
         </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{3D44D06F-E279-4E97-8C92-4CAE468B332E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">"ROUTE"
+- คอลัมน์สำคัญ
+- ห้ามแก้ไขชื่อคอลัมน์
 </t>
         </r>
-      </text>
-    </comment>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{B4B93DC4-BCDE-40B3-9574-79455FBB37DB}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>- ความยาวของข้อมูลห้ามเกิน 12 ตัวอักษร</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{E2712ED5-B625-4FAB-B714-693610E7D57A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -668,7 +684,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{77CA808C-539E-4211-959E-B7263C5EC9A8}">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{A14F1DF2-DC51-4AA5-B9B2-148699010651}">
       <text>
         <r>
           <rPr>
@@ -694,7 +710,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{78E6D9BF-7E01-4FF6-A554-9A625337D3AD}">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{7FE4B928-51CD-47A9-BEF4-5E619C158F78}">
       <text>
         <r>
           <rPr>
@@ -731,7 +747,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{AFB4E436-F703-499C-AFC0-F3A5DE9D4136}">
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{E7A39EFE-EC99-456E-8A8A-C67435829E6E}">
       <text>
         <r>
           <rPr>
@@ -757,7 +773,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{CB409F98-C149-4AC6-A676-C732D799C65B}">
+    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{9042530B-341B-4FF7-B28B-25CDB71516E7}">
       <text>
         <r>
           <rPr>
@@ -783,7 +799,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{E2FD5675-9518-48EF-B0B4-0243398AFAC8}">
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{32FFD05A-EFF0-4348-9CC6-9FF0BF698F27}">
       <text>
         <r>
           <rPr>
@@ -806,11 +822,12 @@
           </rPr>
           <t xml:space="preserve">
 - ใช้สำหรับใส่วันที่เริ่มงาน
-- รูปแบบวันที่: ดด/วว/ปป เช่น 26/09/2024</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{F8DE4E9F-898A-459B-9D74-E96DF9FEC1A4}">
+- รูปแบบวันที่:
+o วันที่-เดือนย่อ-ปี (01-Feb-2024)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{AE160751-43F7-4F77-A2FE-96C6E61EFBF6}">
       <text>
         <r>
           <rPr>
@@ -833,155 +850,148 @@
           </rPr>
           <t xml:space="preserve">
 - ใช้สำหรับใส่วันที่สิ้นสุดงาน
-- รูปแบบวันที่: ดด/วว/ปป เช่น 26/09/2024</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
+- รูปแบบวันที่: 
+o วันที่-เดือนย่อ-ปี (01-Dec-2024)  </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{C2AAC843-98A8-4400-8BE5-59B837DEFB6C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>"SUPERVISOR"
+- คอลัมน์สำคัญ
+- ห้ามแก้ไขชื่อคอลัมน์</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+- ใช้สำหรับใส่จำนวนผู้ควบคุมงาน (Supervisor)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{2B7DB0AF-659D-4FE4-B714-5C80F5B974F8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>"FOREMAN"
+- คอลัมน์สำคัญ
+- ห้ามแก้ไขชื่อคอลัมน์</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+- ใช้สำหรับใส่จำนวนหัวหน้างาน (Foreman)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{0F22F63E-A23E-460F-8874-CAF452E7D8EE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>"SKILL"
+- คอลัมน์สำคัญ
+- ห้ามแก้ไขชื่อคอลัมน์</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+- ใช้สำหรับใส่จำนวน skill</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{22E698F1-F25D-428C-923D-755B1F5CC15F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>"ประเภทของ_PERMIT_TO_WORK"
+- คอลัมน์สำคัญ
+- ห้ามแก้ไขชื่อคอลัมน์</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+- ใช้สำหรับใส่ข้อมูลประเภทของใบอนุญาตทำงาน (PTW)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{0CE0D4C2-62C4-4B60-AAB8-A7452EF1CA8C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>"TYPE"
+- คอลัมน์สำคัญ
+- ห้ามแก้ไขชื่อคอลัมน์</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+- ใช้สำหรับใส่ข้อมูลประเภทของงาน
+- ระบุ TYPE โดยมีตัวเลือกดังนี้
+o ME: เครื่องกล
+o EE: ไฟฟ้า
+o CV: โยธา
+o IC: Instrument &amp; Control
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{D3274338-FD9C-4A3B-99A7-20110654B85E}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>"SUPERVISOR"
-- คอลัมน์สำคัญ
-- ห้ามแก้ไขชื่อคอลัมน์</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-- ใช้สำหรับใส่จำนวนผู้ควบคุมงาน (Supervisor)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{E731BF2A-82DB-4CB0-BA7E-4030527D63A2}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>"FOREMAN"
-- คอลัมน์สำคัญ
-- ห้ามแก้ไขชื่อคอลัมน์</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-- ใช้สำหรับใส่จำนวนหัวหน้างาน (Foreman)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{3EEDCB61-AE27-4DB5-8FD8-9ADBD4D54A9C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>"SKILL"
-- คอลัมน์สำคัญ
-- ห้ามแก้ไขชื่อคอลัมน์</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-- ใช้สำหรับใส่จำนวน skill</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{67AB6315-76E4-49EF-A257-8421E6729AC2}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>"ประเภทของ_PERMIT_TO_WORK"
-- คอลัมน์สำคัญ
-- ห้ามแก้ไขชื่อคอลัมน์</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-- ใช้สำหรับใส่ข้อมูลประเภทของใบอนุญาตทำงาน (PTW)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{54175C78-473C-41DC-9277-8D3F996B5C8A}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>"TYPE"
-- คอลัมน์สำคัญ
-- ห้ามแก้ไขชื่อคอลัมน์</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-- ใช้สำหรับใส่ข้อมูลประเภทของงาน
-- รูปแบบ:
-M : งานเกี่ยวกับเครื่องกล
-E : งานเกี่ยวกับไฟฟ้า
-C : งานเกี่ยวกับโยธา</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{E1987D67-E125-4ED2-A1FB-6CC8A2B9D38D}">
+    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{1B59EEEF-9993-40DC-A81A-DA982640F8C1}">
       <text>
         <r>
           <rPr>
@@ -992,7 +1002,8 @@
             <family val="2"/>
           </rPr>
           <t>"COMMENT"
-- คอลัมน์สำคัญ</t>
+- คอลัมน์สำคัญ
+- ห้ามแก้ไขชื่อคอลัมน์</t>
         </r>
         <r>
           <rPr>
@@ -1011,7 +1022,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>อัตรากำลัง (จำนวนคน)</t>
   </si>
@@ -1115,18 +1126,6 @@
 โดยใส่ 'PTW งานทั่วไป' ไว้ด้านหน้าเสมอ เช่น PTW งานทั่วไป, งานเกี่ยวกับไฟฟ้า</t>
   </si>
   <si>
-    <t>กรอก FINISH DATE ตามรูปแบบดังนี้
-1. วันที่-เดือนย่อ-ปี (01-Dec-2024)  
-2. วันที่/เดือน/ปี (01/12/2024)  
-3. เดือน/วันที่/ปี (12/01/2024)</t>
-  </si>
-  <si>
-    <t>กรอก START DATE ตามรูปแบบดังนี้
-1. วันที่-เดือนย่อ-ปี (01-Feb-2024)  
-2. วันที่/เดือน/ปี (01/02/2024)  
-3. เดือน/วันที่/ปี (02/01/2024)</t>
-  </si>
-  <si>
     <t>กรอก DURATION (HR.)</t>
   </si>
   <si>
@@ -1169,6 +1168,39 @@
   </si>
   <si>
     <t>กรอกค่า SKILL RATE เฉพาะเมื่อ TASK ORDER เท่ากับ 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">กรอก START DATE ตามรูปแบบนี้
+-&gt; วันที่-เดือนย่อ-ปี (01-Feb-2024) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">กรอก FINISH DATE ตามรูปแบบนี้
+-&gt; วันที่-เดือนย่อ-ปี (01-Dec-2024)  </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="TH SarabunPSK"/>
+        <family val="2"/>
+      </rPr>
+      <t>คำแนะนำ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="TH SarabunPSK"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+- ห้ามรวมเซลล์ใน Excel เพื่อป้องกันความผิดพลาดในการดึงข้อมูล
+- ให้ sheet สำหรับประมวลผลอยู่ลำดับแรก</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1178,7 +1210,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1302,13 +1334,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri"/>
@@ -1406,7 +1431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1458,15 +1483,18 @@
     <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1880,26 +1908,28 @@
   <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="1" max="1" width="62.6640625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.6640625" customWidth="1"/>
     <col min="5" max="5" width="42" customWidth="1"/>
-    <col min="6" max="6" width="24.77734375" customWidth="1"/>
-    <col min="7" max="8" width="15.21875" customWidth="1"/>
+    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="45" customWidth="1"/>
     <col min="10" max="10" width="14.5546875" customWidth="1"/>
     <col min="11" max="11" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="26.88671875" customWidth="1"/>
+    <col min="13" max="13" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="15" max="17" width="13.44140625" customWidth="1"/>
     <col min="18" max="18" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.33203125" customWidth="1"/>
+    <col min="19" max="19" width="19.33203125" customWidth="1"/>
     <col min="20" max="20" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1929,7 +1959,7 @@
       <c r="S1" s="11"/>
       <c r="T1" s="12"/>
     </row>
-    <row r="2" spans="1:20" ht="42" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>12</v>
       </c>
@@ -1993,60 +2023,63 @@
     </row>
     <row r="10" spans="1:20" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D10" s="20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="R10" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:20" s="19" customFormat="1" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="23" t="s">
+        <v>41</v>
+      </c>
       <c r="D11" s="19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="O11" s="22" t="s">
         <v>38</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="L11" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="M11" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="N11" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="O11" s="22" t="s">
-        <v>40</v>
       </c>
       <c r="P11" s="22"/>
       <c r="Q11" s="22"/>

</xml_diff>